<commit_message>
table: add id, egpu date, salary date
</commit_message>
<xml_diff>
--- a/Forms/Templates/ExportLoanClient.xlsx
+++ b/Forms/Templates/ExportLoanClient.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">&lt;#RowNumberTitle#&gt;</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">&lt;#ClientTitleTitle#&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;#RoleTitleTitle#&gt;</t>
   </si>
   <si>
@@ -191,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;%ClientTitle%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%LoanClientId%&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;%RoleTitle%&gt;</t>
@@ -770,7 +776,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AW9"/>
+  <dimension ref="A1:AX9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
@@ -784,21 +790,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="8" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="25" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="37" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="41" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="9" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="26" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="38" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="42" style="1" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -835,7 +841,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -871,29 +877,31 @@
       <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5"/>
+      <c r="Y1" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
-      <c r="AE1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="AG1" s="5"/>
       <c r="AH1" s="5"/>
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
-      <c r="AM1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="AO1" s="5"/>
       <c r="AP1" s="5"/>
       <c r="AQ1" s="5"/>
@@ -901,11 +909,12 @@
       <c r="AS1" s="5"/>
       <c r="AT1" s="5"/>
       <c r="AU1" s="5"/>
-      <c r="AV1" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="AV1" s="5"/>
       <c r="AW1" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -920,7 +929,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="4"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -932,9 +941,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
-      <c r="X2" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="X2" s="4"/>
       <c r="Y2" s="4" t="s">
         <v>29</v>
       </c>
@@ -1004,156 +1011,162 @@
       <c r="AU2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AV2" s="4"/>
+      <c r="AV2" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="9" t="s">
         <v>59</v>
       </c>
+      <c r="H3" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="I3" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="O3" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="P3" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="V3" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="V3" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="W3" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="X3" s="8" t="s">
         <v>75</v>
       </c>
+      <c r="X3" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="Y3" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA3" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="AA3" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="AB3" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AC3" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD3" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AF3" s="10" t="s">
+      <c r="AE3" s="10" t="s">
         <v>83</v>
       </c>
+      <c r="AF3" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="AG3" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AH3" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK3" s="8" t="s">
         <v>88</v>
       </c>
+      <c r="AK3" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="AL3" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AM3" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AN3" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO3" s="10" t="s">
         <v>92</v>
       </c>
+      <c r="AO3" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="AP3" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AR3" s="10" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AT3" s="10" t="s">
+      <c r="AS3" s="10" t="s">
         <v>97</v>
       </c>
+      <c r="AT3" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="AU3" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AV3" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AW3" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="AX3" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1164,22 +1177,24 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1203,11 +1218,12 @@
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:AD1"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="AM1:AU1"/>
-    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="AF1:AM1"/>
+    <mergeCell ref="AN1:AV1"/>
     <mergeCell ref="AW1:AW2"/>
+    <mergeCell ref="AX1:AX2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
tablexport: court date, credit date
</commit_message>
<xml_diff>
--- a/Forms/Templates/ExportLoanClient.xlsx
+++ b/Forms/Templates/ExportLoanClient.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t xml:space="preserve">&lt;#RowNumberTitle#&gt;</t>
   </si>
@@ -94,6 +94,9 @@
     <t xml:space="preserve">&lt;#BankruptCheckDateTitle#&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Дата КД</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;#SuccessionTitle#&gt;</t>
   </si>
   <si>
@@ -251,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;%BankruptCheckDate%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%CreditDate%&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;%SuccessionCourtTitle%&gt;</t>
@@ -335,11 +341,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -463,7 +470,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,6 +521,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -776,12 +787,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX9"/>
+  <dimension ref="A1:AY9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="5" ySplit="0" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="Z3" activeCellId="0" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -797,14 +808,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="26" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="38" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="42" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="27" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="34" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="37" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="39" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="43" style="1" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -880,29 +892,31 @@
       <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5"/>
+      <c r="Z1" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
       <c r="AE1" s="5"/>
-      <c r="AF1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="AH1" s="5"/>
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
-      <c r="AN1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AO1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="AP1" s="5"/>
       <c r="AQ1" s="5"/>
       <c r="AR1" s="5"/>
@@ -910,11 +924,12 @@
       <c r="AT1" s="5"/>
       <c r="AU1" s="5"/>
       <c r="AV1" s="5"/>
-      <c r="AW1" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="AW1" s="5"/>
       <c r="AX1" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -942,9 +957,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
-      <c r="Y2" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="Y2" s="4"/>
       <c r="Z2" s="4" t="s">
         <v>30</v>
       </c>
@@ -1014,159 +1027,165 @@
       <c r="AV2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AW2" s="4"/>
+      <c r="AW2" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y3" s="8" t="s">
         <v>77</v>
       </c>
+      <c r="Y3" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="Z3" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB3" s="10" t="s">
         <v>80</v>
       </c>
+      <c r="AB3" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="AC3" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AD3" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AF3" s="10" t="s">
         <v>85</v>
       </c>
+      <c r="AG3" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="AH3" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AK3" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL3" s="8" t="s">
         <v>90</v>
       </c>
+      <c r="AL3" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="AM3" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AN3" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AO3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AP3" s="10" t="s">
         <v>94</v>
       </c>
+      <c r="AP3" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="AQ3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AS3" s="10" t="s">
+      <c r="AR3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AU3" s="10" t="s">
+      <c r="AT3" s="10" t="s">
         <v>99</v>
       </c>
+      <c r="AU3" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="AV3" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AW3" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AX3" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1178,23 +1197,24 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
+      <c r="Y4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1219,11 +1239,12 @@
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="AF1:AM1"/>
-    <mergeCell ref="AN1:AV1"/>
-    <mergeCell ref="AW1:AW2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AW1"/>
     <mergeCell ref="AX1:AX2"/>
+    <mergeCell ref="AY1:AY2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
table: add bailiff title, add epgu comment to export
</commit_message>
<xml_diff>
--- a/Forms/Templates/ExportLoanClient.xlsx
+++ b/Forms/Templates/ExportLoanClient.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t xml:space="preserve">&lt;#RowNumberTitle#&gt;</t>
   </si>
@@ -97,6 +97,12 @@
     <t xml:space="preserve">Дата КД</t>
   </si>
   <si>
+    <t xml:space="preserve">Запрос ЕПГУ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ФИО пристава</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;#SuccessionTitle#&gt;</t>
   </si>
   <si>
@@ -257,6 +263,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;%CreditDate%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%TsEgpuComment%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%BailiffTitle%&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;%SuccessionCourtTitle%&gt;</t>
@@ -787,12 +799,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AY9"/>
+  <dimension ref="A1:BA9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="0" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <pane xSplit="5" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Z3" activeCellId="0" sqref="Z3"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -809,14 +821,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="20.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="27" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="34" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="37" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="39" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="43" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="26" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="29" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="41" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="45" style="1" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -895,41 +907,47 @@
       <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
       <c r="AE1" s="5"/>
       <c r="AF1" s="5"/>
-      <c r="AG1" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="AG1" s="5"/>
       <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
+      <c r="AI1" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
       <c r="AN1" s="5"/>
-      <c r="AO1" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="AO1" s="5"/>
       <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
+      <c r="AQ1" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="AR1" s="5"/>
       <c r="AS1" s="5"/>
       <c r="AT1" s="5"/>
       <c r="AU1" s="5"/>
       <c r="AV1" s="5"/>
       <c r="AW1" s="5"/>
-      <c r="AX1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AY1" s="4" t="s">
-        <v>29</v>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -958,12 +976,8 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
-      <c r="Z2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
       <c r="AB2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1030,162 +1044,174 @@
       <c r="AW2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
+      <c r="AX2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA3" s="8" t="s">
         <v>80</v>
       </c>
+      <c r="Z3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="AB3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD3" s="10" t="s">
         <v>83</v>
       </c>
+      <c r="AC3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD3" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="AE3" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG3" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="AH3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI3" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="AI3" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AK3" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AL3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM3" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN3" s="8" t="s">
         <v>93</v>
       </c>
+      <c r="AM3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN3" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="AO3" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AP3" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>98</v>
       </c>
+      <c r="AR3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS3" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="AT3" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AU3" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AV3" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW3" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="AW3" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="AX3" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AY3" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="AZ3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1198,6 +1224,8 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E5" s="14"/>
@@ -1214,7 +1242,7 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1240,11 +1268,13 @@
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AW1"/>
-    <mergeCell ref="AX1:AX2"/>
-    <mergeCell ref="AY1:AY2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AH1"/>
+    <mergeCell ref="AI1:AP1"/>
+    <mergeCell ref="AQ1:AY1"/>
+    <mergeCell ref="AZ1:AZ2"/>
+    <mergeCell ref="BA1:BA2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>